<commit_message>
add daily_temperature.py and modify xlsx
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaodanny/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaodanny/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1C3A1E-CA58-E846-8CB5-9241365C8391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCFDE07-9BD7-2A4D-B94E-505D0185B6B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28260" windowHeight="16020" activeTab="1" xr2:uid="{229FDA82-3672-0941-ABC4-BD05A6EE4559}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="248">
   <si>
     <t>two sum 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1010,6 +1010,34 @@
   </si>
   <si>
     <t>Use OrderedDict to do get and put function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Daily Temperatures</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use stack to deal with this , remember to store position rather han value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/daily-temperatures/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use DP to finish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1991,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DC4C1F-E314-1A4C-B8C5-7E3C57124099}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -3371,6 +3399,55 @@
       </c>
       <c r="H59" s="39" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="14">
+        <v>739</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="16">
+        <v>2</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="H60" s="39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="14">
+        <v>64</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" s="16">
+        <v>2</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="H61" s="39" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3434,6 +3511,8 @@
     <hyperlink ref="H57" r:id="rId56" xr:uid="{DE412784-118A-104A-B060-66D3B16DDADA}"/>
     <hyperlink ref="H58" r:id="rId57" xr:uid="{A8A9EABD-B037-FF4E-BB40-E2FE11F09AEB}"/>
     <hyperlink ref="H59" r:id="rId58" xr:uid="{7B1D76D7-3971-644C-9C01-39CA0673DA2B}"/>
+    <hyperlink ref="H60" r:id="rId59" xr:uid="{A46F5914-13C2-744D-ADF6-3CFD7A67EAB5}"/>
+    <hyperlink ref="H61" r:id="rId60" xr:uid="{6F35B688-1AD2-584F-880B-A4F84DC1FD84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>